<commit_message>
Add effort-squared to all regression models.
</commit_message>
<xml_diff>
--- a/output/20221115/tables/effort/betas_hh.xlsx
+++ b/output/20221115/tables/effort/betas_hh.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="18">
   <si>
     <t>Outcome</t>
   </si>
@@ -184,10 +184,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="1">
-        <v>0.38143458962440491</v>
+        <v>0.38436940312385559</v>
       </c>
       <c r="E3" s="1">
-        <v>0.078820571303367615</v>
+        <v>0.078547939658164978</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -196,10 +196,10 @@
         <v>15</v>
       </c>
       <c r="H3" s="1">
-        <v>0.22694626450538635</v>
+        <v>0.23041544854640961</v>
       </c>
       <c r="I3" s="1">
-        <v>0.53592288494110107</v>
+        <v>0.53832334280014038</v>
       </c>
     </row>
     <row r="4">
@@ -213,10 +213,10 @@
         <v>9</v>
       </c>
       <c r="D4" s="1">
-        <v>0.39644512534141541</v>
+        <v>0.39489689469337463</v>
       </c>
       <c r="E4" s="1">
-        <v>0.07859821617603302</v>
+        <v>0.078298427164554596</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
@@ -225,10 +225,10 @@
         <v>15</v>
       </c>
       <c r="H4" s="1">
-        <v>0.24239261448383331</v>
+        <v>0.24143198132514954</v>
       </c>
       <c r="I4" s="1">
-        <v>0.55049765110015869</v>
+        <v>0.54836183786392212</v>
       </c>
     </row>
     <row r="5">
@@ -242,10 +242,10 @@
         <v>10</v>
       </c>
       <c r="D5" s="1">
-        <v>0.4135589599609375</v>
+        <v>0.41082605719566345</v>
       </c>
       <c r="E5" s="1">
-        <v>0.072071172297000885</v>
+        <v>0.072752475738525391</v>
       </c>
       <c r="F5" t="s">
         <v>5</v>
@@ -254,10 +254,10 @@
         <v>15</v>
       </c>
       <c r="H5" s="1">
-        <v>0.27229946851730347</v>
+        <v>0.26823121309280396</v>
       </c>
       <c r="I5" s="1">
-        <v>0.55481845140457153</v>
+        <v>0.55342090129852295</v>
       </c>
     </row>
     <row r="6">
@@ -300,10 +300,10 @@
         <v>8</v>
       </c>
       <c r="D7" s="1">
-        <v>0.89680230617523193</v>
+        <v>0.89445489645004272</v>
       </c>
       <c r="E7" s="1">
-        <v>0.016864331439137459</v>
+        <v>0.018512062728404999</v>
       </c>
       <c r="F7" t="s">
         <v>1</v>
@@ -312,10 +312,10 @@
         <v>15</v>
       </c>
       <c r="H7" s="1">
-        <v>0.86374819278717041</v>
+        <v>0.85817122459411621</v>
       </c>
       <c r="I7" s="1">
-        <v>0.92985641956329346</v>
+        <v>0.93073856830596924</v>
       </c>
     </row>
     <row r="8">
@@ -329,10 +329,10 @@
         <v>9</v>
       </c>
       <c r="D8" s="1">
-        <v>0.89658713340759277</v>
+        <v>0.89466220140457153</v>
       </c>
       <c r="E8" s="1">
-        <v>0.015825795009732246</v>
+        <v>0.01751946285367012</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
@@ -341,10 +341,10 @@
         <v>15</v>
       </c>
       <c r="H8" s="1">
-        <v>0.86556857824325562</v>
+        <v>0.86032402515411377</v>
       </c>
       <c r="I8" s="1">
-        <v>0.92760568857192993</v>
+        <v>0.9290003776550293</v>
       </c>
     </row>
     <row r="9">
@@ -358,10 +358,10 @@
         <v>10</v>
       </c>
       <c r="D9" s="1">
-        <v>0.89520347118377686</v>
+        <v>0.89355921745300293</v>
       </c>
       <c r="E9" s="1">
-        <v>0.01529624592512846</v>
+        <v>0.016960123553872108</v>
       </c>
       <c r="F9" t="s">
         <v>1</v>
@@ -370,10 +370,10 @@
         <v>15</v>
       </c>
       <c r="H9" s="1">
-        <v>0.86522281169891357</v>
+        <v>0.86031734943389893</v>
       </c>
       <c r="I9" s="1">
-        <v>0.92518413066864014</v>
+        <v>0.92680108547210693</v>
       </c>
     </row>
     <row r="10">
@@ -416,10 +416,10 @@
         <v>8</v>
       </c>
       <c r="D11" s="1">
-        <v>0.2285275012254715</v>
+        <v>0.23652034997940063</v>
       </c>
       <c r="E11" s="1">
-        <v>0.030858660116791725</v>
+        <v>0.032814193516969681</v>
       </c>
       <c r="F11" t="s">
         <v>1</v>
@@ -428,10 +428,10 @@
         <v>15</v>
       </c>
       <c r="H11" s="1">
-        <v>0.16804452240467072</v>
+        <v>0.17220452427864075</v>
       </c>
       <c r="I11" s="1">
-        <v>0.28901046514511108</v>
+        <v>0.30083617568016052</v>
       </c>
     </row>
     <row r="12">
@@ -445,10 +445,10 @@
         <v>9</v>
       </c>
       <c r="D12" s="1">
-        <v>0.23231123387813568</v>
+        <v>0.24002310633659363</v>
       </c>
       <c r="E12" s="1">
-        <v>0.028539864346385002</v>
+        <v>0.030129756778478622</v>
       </c>
       <c r="F12" t="s">
         <v>1</v>
@@ -457,10 +457,10 @@
         <v>15</v>
       </c>
       <c r="H12" s="1">
-        <v>0.17637309432029724</v>
+        <v>0.18096877634525299</v>
       </c>
       <c r="I12" s="1">
-        <v>0.28824937343597412</v>
+        <v>0.29907742142677307</v>
       </c>
     </row>
     <row r="13">
@@ -474,10 +474,10 @@
         <v>10</v>
       </c>
       <c r="D13" s="1">
-        <v>0.23629799485206604</v>
+        <v>0.24305523931980133</v>
       </c>
       <c r="E13" s="1">
-        <v>0.030110163614153862</v>
+        <v>0.031533610075712204</v>
       </c>
       <c r="F13" t="s">
         <v>1</v>
@@ -486,10 +486,10 @@
         <v>15</v>
       </c>
       <c r="H13" s="1">
-        <v>0.17728208005428314</v>
+        <v>0.18124936521053314</v>
       </c>
       <c r="I13" s="1">
-        <v>0.29531392455101013</v>
+        <v>0.30486112833023071</v>
       </c>
     </row>
     <row r="14">
@@ -532,10 +532,10 @@
         <v>8</v>
       </c>
       <c r="D15" s="1">
-        <v>0.32744944095611572</v>
+        <v>0.3303561806678772</v>
       </c>
       <c r="E15" s="1">
-        <v>0.069241061806678772</v>
+        <v>0.068532422184944153</v>
       </c>
       <c r="F15" t="s">
         <v>5</v>
@@ -544,10 +544,10 @@
         <v>15</v>
       </c>
       <c r="H15" s="1">
-        <v>0.19173696637153625</v>
+        <v>0.19603262841701508</v>
       </c>
       <c r="I15" s="1">
-        <v>0.46316191554069519</v>
+        <v>0.46467971801757812</v>
       </c>
     </row>
     <row r="16">
@@ -561,10 +561,10 @@
         <v>9</v>
       </c>
       <c r="D16" s="1">
-        <v>0.34423094987869263</v>
+        <v>0.34271252155303955</v>
       </c>
       <c r="E16" s="1">
-        <v>0.067337781190872192</v>
+        <v>0.066865712404251099</v>
       </c>
       <c r="F16" t="s">
         <v>5</v>
@@ -573,10 +573,10 @@
         <v>15</v>
       </c>
       <c r="H16" s="1">
-        <v>0.21224889159202576</v>
+        <v>0.21165572106838226</v>
       </c>
       <c r="I16" s="1">
-        <v>0.4762130081653595</v>
+        <v>0.47376930713653564</v>
       </c>
     </row>
     <row r="17">
@@ -590,10 +590,10 @@
         <v>10</v>
       </c>
       <c r="D17" s="1">
-        <v>0.3604724109172821</v>
+        <v>0.35777807235717773</v>
       </c>
       <c r="E17" s="1">
-        <v>0.060195032507181168</v>
+        <v>0.060750715434551239</v>
       </c>
       <c r="F17" t="s">
         <v>5</v>
@@ -602,10 +602,10 @@
         <v>15</v>
       </c>
       <c r="H17" s="1">
-        <v>0.24249014258384705</v>
+        <v>0.23870666325092316</v>
       </c>
       <c r="I17" s="1">
-        <v>0.47845467925071716</v>
+        <v>0.47684946656227112</v>
       </c>
     </row>
     <row r="18">
@@ -648,10 +648,10 @@
         <v>8</v>
       </c>
       <c r="D19" s="1">
-        <v>0.077044472098350525</v>
+        <v>0.076747387647628784</v>
       </c>
       <c r="E19" s="1">
-        <v>0.031488746404647827</v>
+        <v>0.031236883252859116</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
@@ -660,10 +660,10 @@
         <v>15</v>
       </c>
       <c r="H19" s="1">
-        <v>0.015326528809964657</v>
+        <v>0.015523096546530724</v>
       </c>
       <c r="I19" s="1">
-        <v>0.13876241445541382</v>
+        <v>0.13797168433666229</v>
       </c>
     </row>
     <row r="20">
@@ -677,10 +677,10 @@
         <v>9</v>
       </c>
       <c r="D20" s="1">
-        <v>0.071495316922664642</v>
+        <v>0.071647018194198608</v>
       </c>
       <c r="E20" s="1">
-        <v>0.031987257301807404</v>
+        <v>0.032153081148862839</v>
       </c>
       <c r="F20" t="s">
         <v>5</v>
@@ -689,10 +689,10 @@
         <v>15</v>
       </c>
       <c r="H20" s="1">
-        <v>0.0088002923876047134</v>
+        <v>0.0086269788444042206</v>
       </c>
       <c r="I20" s="1">
-        <v>0.13419033586978912</v>
+        <v>0.1346670538187027</v>
       </c>
     </row>
     <row r="21">
@@ -706,10 +706,10 @@
         <v>10</v>
       </c>
       <c r="D21" s="1">
-        <v>0.072180032730102539</v>
+        <v>0.072508752346038818</v>
       </c>
       <c r="E21" s="1">
-        <v>0.032154947519302368</v>
+        <v>0.032341912388801575</v>
       </c>
       <c r="F21" t="s">
         <v>5</v>
@@ -718,10 +718,10 @@
         <v>15</v>
       </c>
       <c r="H21" s="1">
-        <v>0.0091563351452350616</v>
+        <v>0.0091186044737696648</v>
       </c>
       <c r="I21" s="1">
-        <v>0.13520373404026031</v>
+        <v>0.1358989030122757</v>
       </c>
     </row>
   </sheetData>

</xml_diff>